<commit_message>
Add more data, tidy up some soil settings
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observations/RS14_15_Biomass.xlsx
+++ b/Prototypes/Barley/Observations/RS14_15_Biomass.xlsx
@@ -438,12 +438,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Fixed RS1415 final harvest results, bad calculations in original data sheet
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observations/RS14_15_Biomass.xlsx
+++ b/Prototypes/Barley/Observations/RS14_15_Biomass.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26:N31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,28 +1268,28 @@
         <v>42046</v>
       </c>
       <c r="C26">
-        <v>2384.1069969462137</v>
+        <v>2400.2938700802683</v>
       </c>
       <c r="E26">
-        <v>699.46641981008599</v>
+        <v>704.22882872714194</v>
       </c>
       <c r="F26">
-        <v>145.29608662616897</v>
+        <v>146.2989190295223</v>
       </c>
       <c r="G26">
-        <v>1539.3444905099586</v>
+        <v>1196.675294936432</v>
       </c>
       <c r="I26">
         <v>1207.8518076133</v>
       </c>
       <c r="K26">
-        <v>3.7923821250000003E-2</v>
+        <v>3.3250441271250007E-2</v>
       </c>
       <c r="L26">
-        <v>34211.679628737176</v>
+        <v>31358.030921863901</v>
       </c>
       <c r="M26">
-        <v>1297.4376229024951</v>
+        <v>1042.6683655494774</v>
       </c>
       <c r="N26" t="s">
         <v>14</v>
@@ -1303,28 +1303,28 @@
         <v>42032</v>
       </c>
       <c r="C27">
-        <v>1309.4161577956536</v>
+        <v>1316.8943799147532</v>
       </c>
       <c r="E27">
-        <v>333.48139256810322</v>
+        <v>335.38560674653718</v>
       </c>
       <c r="F27">
-        <v>68.490579495842752</v>
+        <v>68.882027387918328</v>
       </c>
       <c r="G27">
-        <v>907.44418573170765</v>
+        <v>726.6255744620322</v>
       </c>
       <c r="I27">
         <v>921.56699574098207</v>
       </c>
       <c r="K27">
-        <v>3.1291507499999996E-2</v>
+        <v>2.7450779798749995E-2</v>
       </c>
       <c r="L27">
-        <v>22612.278074611455</v>
+        <v>21720.636897403987</v>
       </c>
       <c r="M27">
-        <v>707.57226896378984</v>
+        <v>596.24842055924114</v>
       </c>
       <c r="N27" t="s">
         <v>14</v>
@@ -1338,28 +1338,28 @@
         <v>42046</v>
       </c>
       <c r="C28">
-        <v>1368.3650200206234</v>
+        <v>1370.7322634204334</v>
       </c>
       <c r="E28">
-        <v>332.87369480662585</v>
+        <v>333.45080520281903</v>
       </c>
       <c r="F28">
-        <v>54.149533821533247</v>
+        <v>54.245145438268899</v>
       </c>
       <c r="G28">
-        <v>981.3417913924643</v>
+        <v>906.31477357120059</v>
       </c>
       <c r="I28">
         <v>962.80860878677345</v>
       </c>
       <c r="K28">
-        <v>3.6951699375000001E-2</v>
+        <v>3.250710120375E-2</v>
       </c>
       <c r="L28">
-        <v>22443.701905376849</v>
+        <v>24271.490366281625</v>
       </c>
       <c r="M28">
-        <v>829.33292566960006</v>
+        <v>788.99579370255992</v>
       </c>
       <c r="N28" t="s">
         <v>14</v>
@@ -1373,28 +1373,28 @@
         <v>42046</v>
       </c>
       <c r="C29">
-        <v>2075.388390982424</v>
+        <v>2087.5735007623325</v>
       </c>
       <c r="E29">
-        <v>666.78442965503268</v>
+        <v>670.763347186695</v>
       </c>
       <c r="F29">
-        <v>131.05061928528255</v>
+        <v>131.89723230104508</v>
       </c>
       <c r="G29">
-        <v>1277.5533420421084</v>
+        <v>989.84963015370579</v>
       </c>
       <c r="I29">
         <v>942.24292925521945</v>
       </c>
       <c r="K29">
-        <v>3.9966151875000001E-2</v>
+        <v>3.5086588213125006E-2</v>
       </c>
       <c r="L29">
-        <v>24705.726938645974</v>
+        <v>22894.089091506761</v>
       </c>
       <c r="M29">
-        <v>987.39283501220382</v>
+        <v>803.27547646829487</v>
       </c>
       <c r="N29" t="s">
         <v>14</v>
@@ -1408,28 +1408,28 @@
         <v>42032</v>
       </c>
       <c r="C30">
-        <v>1413.111329121356</v>
+        <v>1420.4325771695444</v>
       </c>
       <c r="E30">
-        <v>406.5457527734826</v>
+        <v>408.64344656098058</v>
       </c>
       <c r="F30">
-        <v>91.973460479881879</v>
+        <v>92.449333186439617</v>
       </c>
       <c r="G30">
-        <v>914.59211586799177</v>
+        <v>737.28406209330058</v>
       </c>
       <c r="I30">
         <v>882.48157752299119</v>
       </c>
       <c r="K30">
-        <v>3.1759653749999998E-2</v>
+        <v>2.7773201774999996E-2</v>
       </c>
       <c r="L30">
-        <v>20870.560530061066</v>
+        <v>20184.601146307563</v>
       </c>
       <c r="M30">
-        <v>662.84177600315593</v>
+        <v>560.59100038429619</v>
       </c>
       <c r="N30" t="s">
         <v>14</v>
@@ -1443,28 +1443,28 @@
         <v>42046</v>
       </c>
       <c r="C31">
-        <v>1397.7103613422337</v>
+        <v>1399.6031274815796</v>
       </c>
       <c r="E31">
-        <v>369.52710959120782</v>
+        <v>370.0282563280702</v>
       </c>
       <c r="F31">
-        <v>56.197526955467403</v>
+        <v>56.273960173709533</v>
       </c>
       <c r="G31">
-        <v>971.98572479555844</v>
+        <v>837.78601328482796</v>
       </c>
       <c r="I31">
         <v>997.94602945182271</v>
       </c>
       <c r="K31">
-        <v>3.9097641249999995E-2</v>
+        <v>3.42295942225E-2</v>
       </c>
       <c r="L31">
-        <v>18574.683868388373</v>
+        <v>20431.203681213374</v>
       </c>
       <c r="M31">
-        <v>726.22632621841069</v>
+        <v>699.351811485182</v>
       </c>
       <c r="N31" t="s">
         <v>14</v>

</xml_diff>